<commit_message>
Add export file feature
</commit_message>
<xml_diff>
--- a/排班.xlsx
+++ b/排班.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Python\Project\auto-excel-schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63AF59E-23AD-467C-BD44-576BDEB318F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CFA63B-040E-4A20-82FA-4D91F98C440E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="43">
   <si>
     <t>星  期</t>
   </si>
@@ -459,6 +459,10 @@
       </rPr>
       <t>表示倒班</t>
     </r>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>白班家里面有点事情处理</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
 </sst>
@@ -844,6 +848,9 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -859,6 +866,9 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -866,12 +876,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1184,7 +1188,7 @@
   <dimension ref="A1:AG22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection sqref="A1:AG1"/>
+      <selection activeCell="AD11" sqref="AD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
@@ -1200,41 +1204,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="47.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="23"/>
     </row>
     <row r="2" spans="1:33" ht="30.6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
@@ -1533,7 +1537,9 @@
       <c r="AF4" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="AG4" s="14"/>
+      <c r="AG4" s="14" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="5" spans="1:33" ht="26.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
@@ -2893,119 +2899,119 @@
       <c r="AG19" s="14"/>
     </row>
     <row r="20" spans="1:33" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
-      <c r="T20" s="24"/>
-      <c r="U20" s="24"/>
-      <c r="V20" s="24"/>
-      <c r="W20" s="24"/>
-      <c r="X20" s="24"/>
-      <c r="Y20" s="24"/>
-      <c r="Z20" s="24"/>
-      <c r="AA20" s="24"/>
-      <c r="AB20" s="24"/>
-      <c r="AC20" s="24"/>
-      <c r="AD20" s="24"/>
-      <c r="AE20" s="24"/>
-      <c r="AF20" s="24"/>
-      <c r="AG20" s="24"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="25"/>
+      <c r="P20" s="25"/>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="25"/>
+      <c r="S20" s="25"/>
+      <c r="T20" s="25"/>
+      <c r="U20" s="25"/>
+      <c r="V20" s="25"/>
+      <c r="W20" s="25"/>
+      <c r="X20" s="25"/>
+      <c r="Y20" s="25"/>
+      <c r="Z20" s="25"/>
+      <c r="AA20" s="25"/>
+      <c r="AB20" s="25"/>
+      <c r="AC20" s="25"/>
+      <c r="AD20" s="25"/>
+      <c r="AE20" s="25"/>
+      <c r="AF20" s="25"/>
+      <c r="AG20" s="25"/>
     </row>
     <row r="21" spans="1:33" ht="87.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25"/>
-      <c r="O21" s="25"/>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="25"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="25"/>
-      <c r="T21" s="25"/>
-      <c r="U21" s="25"/>
-      <c r="V21" s="25"/>
-      <c r="W21" s="25"/>
-      <c r="X21" s="25"/>
-      <c r="Y21" s="25"/>
-      <c r="Z21" s="25"/>
-      <c r="AA21" s="25"/>
-      <c r="AB21" s="25"/>
-      <c r="AC21" s="25"/>
-      <c r="AD21" s="25"/>
-      <c r="AE21" s="25"/>
-      <c r="AF21" s="25"/>
-      <c r="AG21" s="25"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="26"/>
+      <c r="R21" s="26"/>
+      <c r="S21" s="26"/>
+      <c r="T21" s="26"/>
+      <c r="U21" s="26"/>
+      <c r="V21" s="26"/>
+      <c r="W21" s="26"/>
+      <c r="X21" s="26"/>
+      <c r="Y21" s="26"/>
+      <c r="Z21" s="26"/>
+      <c r="AA21" s="26"/>
+      <c r="AB21" s="26"/>
+      <c r="AC21" s="26"/>
+      <c r="AD21" s="26"/>
+      <c r="AE21" s="26"/>
+      <c r="AF21" s="26"/>
+      <c r="AG21" s="26"/>
     </row>
     <row r="22" spans="1:33" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="27" t="s">
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="26"/>
-      <c r="Q22" s="26"/>
-      <c r="R22" s="26"/>
-      <c r="S22" s="26"/>
-      <c r="T22" s="26"/>
-      <c r="U22" s="26"/>
-      <c r="V22" s="26" t="s">
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="28"/>
+      <c r="P22" s="28"/>
+      <c r="Q22" s="28"/>
+      <c r="R22" s="28"/>
+      <c r="S22" s="28"/>
+      <c r="T22" s="28"/>
+      <c r="U22" s="28"/>
+      <c r="V22" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="W22" s="26"/>
-      <c r="X22" s="26"/>
-      <c r="Y22" s="26"/>
-      <c r="Z22" s="26"/>
-      <c r="AA22" s="26"/>
-      <c r="AB22" s="26"/>
-      <c r="AC22" s="26"/>
-      <c r="AD22" s="26"/>
-      <c r="AE22" s="26"/>
-      <c r="AF22" s="26"/>
-      <c r="AG22" s="28"/>
+      <c r="W22" s="28"/>
+      <c r="X22" s="28"/>
+      <c r="Y22" s="28"/>
+      <c r="Z22" s="28"/>
+      <c r="AA22" s="28"/>
+      <c r="AB22" s="28"/>
+      <c r="AC22" s="28"/>
+      <c r="AD22" s="28"/>
+      <c r="AE22" s="28"/>
+      <c r="AF22" s="28"/>
+      <c r="AG22" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>